<commit_message>
working on building stock generator
</commit_message>
<xml_diff>
--- a/data/residential_model/_EXCELFILES/data_residential_model_dwtype_age.xlsx
+++ b/data/residential_model/_EXCELFILES/data_residential_model_dwtype_age.xlsx
@@ -828,7 +828,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
@@ -922,6 +922,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="%" xfId="5"/>
@@ -2403,11 +2404,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120838400"/>
-        <c:axId val="133201920"/>
+        <c:axId val="69102592"/>
+        <c:axId val="69944448"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="120838400"/>
+        <c:axId val="69102592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,7 +2443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133201920"/>
+        <c:crossAx val="69944448"/>
         <c:crossesAt val="0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2452,7 +2453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133201920"/>
+        <c:axId val="69944448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2498,7 +2499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120838400"/>
+        <c:crossAx val="69102592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2954,11 +2955,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133266432"/>
-        <c:axId val="133276416"/>
+        <c:axId val="98715520"/>
+        <c:axId val="70701056"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="133266432"/>
+        <c:axId val="98715520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2993,7 +2994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133276416"/>
+        <c:crossAx val="70701056"/>
         <c:crossesAt val="0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3002,7 +3003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133276416"/>
+        <c:axId val="70701056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3048,7 +3049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133266432"/>
+        <c:crossAx val="98715520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3472,10 +3473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,6 +3576,26 @@
       </c>
       <c r="F5">
         <v>5.4076118484662032</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>2015</v>
+      </c>
+      <c r="B6" s="35">
+        <v>20.8</v>
+      </c>
+      <c r="C6" s="35">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="D6" s="35">
+        <v>29.5</v>
+      </c>
+      <c r="E6" s="35">
+        <v>8</v>
+      </c>
+      <c r="F6" s="35">
+        <v>5.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>